<commit_message>
Activates JPA errors on embedded ID class with rel. mappings
resume-domain-jpa, resume-persistence-jpa
</commit_message>
<xml_diff>
--- a/PersonalNotes/JPA Errors & warnings.xlsx
+++ b/PersonalNotes/JPA Errors & warnings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dropbox\devArturo\repos\JRebel-Angular\com.tecxis.resume.project\PersonalNotes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{131A49C3-7C27-473F-84C9-2233B0C8AA54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89018391-7451-4039-95FE-2F054620DF2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{5D1D5867-4F85-49F2-A862-98A19BEF0360}"/>
   </bookViews>
@@ -406,7 +406,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -416,6 +416,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -432,9 +438,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -753,7 +760,7 @@
   <dimension ref="A1:B112"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -833,7 +840,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -841,7 +848,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -849,7 +856,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -857,15 +864,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="1" t="s">
+    <row r="13" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B13" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -945,7 +952,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -961,7 +968,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>28</v>
       </c>
@@ -969,7 +976,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>29</v>
       </c>
@@ -985,7 +992,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>31</v>
       </c>
@@ -1017,7 +1024,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>35</v>
       </c>
@@ -1073,7 +1080,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>42</v>
       </c>
@@ -1081,7 +1088,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>43</v>
       </c>
@@ -1105,7 +1112,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>46</v>
       </c>
@@ -1185,7 +1192,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>56</v>
       </c>
@@ -1193,15 +1200,15 @@
         <v>11</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A55" t="s">
+    <row r="55" spans="1:2" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B55" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B55" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>58</v>
       </c>
@@ -1209,7 +1216,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="57" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>59</v>
       </c>
@@ -1249,7 +1256,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="62" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>64</v>
       </c>
@@ -1257,7 +1264,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="63" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>65</v>
       </c>
@@ -1265,7 +1272,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="64" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>66</v>
       </c>
@@ -1273,7 +1280,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="65" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>67</v>
       </c>
@@ -1281,7 +1288,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="66" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>68</v>
       </c>
@@ -1289,7 +1296,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="67" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>69</v>
       </c>
@@ -1409,7 +1416,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>84</v>
       </c>
@@ -1425,7 +1432,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>86</v>
       </c>
@@ -1433,7 +1440,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>87</v>
       </c>
@@ -1441,7 +1448,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="86" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>88</v>
       </c>
@@ -1449,15 +1456,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="87" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A87" t="s">
+    <row r="87" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A87" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B87" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+      <c r="B87" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>90</v>
       </c>
@@ -1465,7 +1472,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>91</v>
       </c>
@@ -1529,7 +1536,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>99</v>
       </c>
@@ -1585,7 +1592,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>106</v>
       </c>
@@ -1593,7 +1600,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>107</v>
       </c>
@@ -1659,9 +1666,26 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:B112" xr:uid="{6874E883-E557-4DD3-BDC7-33FC41A792D5}">
-    <filterColumn colId="1">
+    <filterColumn colId="0">
       <filters>
-        <filter val="ignore"/>
+        <filter val="problem.EMBEDDED_ID_CLASS_SHOULD_BE_PUBLIC"/>
+        <filter val="problem.EMBEDDED_ID_CLASS_SHOULD_IMPLEMENT_SERIALIZABLE"/>
+        <filter val="problem.EMBEDDED_ID_CLASS_SHOULD_NOT_CONTAIN_RELATIONSHIP_MAPPINGS"/>
+        <filter val="problem.PERSISTENCE_UNIT_INVALID_CLASS"/>
+        <filter val="problem.TYPE_MAPPING_ID_CLASS_ATTRIBUTE_DOES_NOT_EXIST"/>
+        <filter val="problem.TYPE_MAPPING_ID_CLASS_ATTRIBUTE_MAPPING_DUPLICATE_MATCH"/>
+        <filter val="problem.TYPE_MAPPING_ID_CLASS_ATTRIBUTE_MAPPING_NO_MATCH"/>
+        <filter val="problem.TYPE_MAPPING_ID_CLASS_ATTRIBUTE_NOT_PRIMARY_KEY"/>
+        <filter val="problem.TYPE_MAPPING_ID_CLASS_ATTRIBUTE_TYPE_DOES_NOT_AGREE"/>
+        <filter val="problem.TYPE_MAPPING_ID_CLASS_MISSING_EQUALS_METHOD"/>
+        <filter val="problem.TYPE_MAPPING_ID_CLASS_MISSING_HASHCODE_METHOD"/>
+        <filter val="problem.TYPE_MAPPING_ID_CLASS_NAME_EMPTY"/>
+        <filter val="problem.TYPE_MAPPING_ID_CLASS_NOT_IMPLEMENT_SERIALIZABLE"/>
+        <filter val="problem.TYPE_MAPPING_ID_CLASS_NOT_PUBLIC"/>
+        <filter val="problem.TYPE_MAPPING_ID_CLASS_PROPERTY_METHOD_NOT_PUBLIC"/>
+        <filter val="problem.VIRTUAL_ATTRIBUTE_EMBEDDED_ID_CLASS_SHOULD_BE_PUBLIC"/>
+        <filter val="problem.VIRTUAL_ATTRIBUTE_EMBEDDED_ID_CLASS_SHOULD_IMPLEMENT_NO_ARG_CONSTRUCTOR"/>
+        <filter val="problem.VIRTUAL_ATTRIBUTE_EMBEDDED_ID_CLASS_SHOULD_NOT_CONTAIN_RELATIONSHIP_MAPPINGS"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
Enables warning (not error) for entity java class members for u. testing
</commit_message>
<xml_diff>
--- a/PersonalNotes/JPA Errors & warnings.xlsx
+++ b/PersonalNotes/JPA Errors & warnings.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dropbox\devArturo\repos\JRebel-Angular\com.tecxis.resume.project\PersonalNotes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dropbox\devArturo\repos\dev\com.tecxis.resume.project\PersonalNotes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89018391-7451-4039-95FE-2F054620DF2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54276DB3-E68F-4A43-9864-516C3A3E1BDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{5D1D5867-4F85-49F2-A862-98A19BEF0360}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$B$112</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$B$113</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="119">
   <si>
     <t>eclipse.preferences.version</t>
   </si>
@@ -391,6 +391,9 @@
   </si>
   <si>
     <t>Code</t>
+  </si>
+  <si>
+    <t>problem.TYPE_MAPPING_MEMBER_CLASS</t>
   </si>
 </sst>
 </file>
@@ -757,10 +760,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6874E883-E557-4DD3-BDC7-33FC41A792D5}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:B112"/>
+  <dimension ref="A1:B113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="A113" sqref="A113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -792,7 +795,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -840,7 +843,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -888,7 +891,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -896,7 +899,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -904,7 +907,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -952,7 +955,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -992,7 +995,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>31</v>
       </c>
@@ -1000,7 +1003,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>32</v>
       </c>
@@ -1040,7 +1043,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>37</v>
       </c>
@@ -1056,7 +1059,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>39</v>
       </c>
@@ -1200,7 +1203,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="55" spans="1:2" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
         <v>57</v>
       </c>
@@ -1440,7 +1443,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="85" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>87</v>
       </c>
@@ -1536,7 +1539,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="97" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>99</v>
       </c>
@@ -1664,14 +1667,33 @@
         <v>1</v>
       </c>
     </row>
+    <row r="113" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A113" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B113" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:B112" xr:uid="{6874E883-E557-4DD3-BDC7-33FC41A792D5}">
+  <autoFilter ref="A1:B113" xr:uid="{6874E883-E557-4DD3-BDC7-33FC41A792D5}">
     <filterColumn colId="0">
       <filters>
+        <filter val="org.eclipse.jpt.jpa.core.discoverAnnotatedClasses"/>
+        <filter val="problem.ELEMENT_COLLECTION_TARGET_CLASS_NOT_DEFINED"/>
         <filter val="problem.EMBEDDED_ID_CLASS_SHOULD_BE_PUBLIC"/>
         <filter val="problem.EMBEDDED_ID_CLASS_SHOULD_IMPLEMENT_SERIALIZABLE"/>
         <filter val="problem.EMBEDDED_ID_CLASS_SHOULD_NOT_CONTAIN_RELATIONSHIP_MAPPINGS"/>
+        <filter val="problem.ENTITY_TABLE_PER_CLASS_DISCRIMINATOR_COLUMN_DEFINED"/>
+        <filter val="problem.ENTITY_TABLE_PER_CLASS_DISCRIMINATOR_VALUE_DEFINED"/>
+        <filter val="problem.ENTITY_TABLE_PER_CLASS_NOT_SUPPORTED_ON_PLATFORM"/>
+        <filter val="problem.MANAGED_TYPE_UNSPECIFIED_CLASS"/>
+        <filter val="problem.MAP_KEY_CLASS_NOT_DEFINED"/>
+        <filter val="problem.MAP_KEY_CLASS_NOT_EXIST"/>
         <filter val="problem.PERSISTENCE_UNIT_INVALID_CLASS"/>
+        <filter val="problem.PERSISTENCE_UNIT_NONEXISTENT_CLASS"/>
+        <filter val="problem.PERSISTENCE_UNIT_UNSPECIFIED_CLASS"/>
+        <filter val="problem.TYPE_MAPPING_CLASS_MISSING_NO_ARG_CONSTRUCTOR"/>
         <filter val="problem.TYPE_MAPPING_ID_CLASS_ATTRIBUTE_DOES_NOT_EXIST"/>
         <filter val="problem.TYPE_MAPPING_ID_CLASS_ATTRIBUTE_MAPPING_DUPLICATE_MATCH"/>
         <filter val="problem.TYPE_MAPPING_ID_CLASS_ATTRIBUTE_MAPPING_NO_MATCH"/>
@@ -1683,9 +1705,12 @@
         <filter val="problem.TYPE_MAPPING_ID_CLASS_NOT_IMPLEMENT_SERIALIZABLE"/>
         <filter val="problem.TYPE_MAPPING_ID_CLASS_NOT_PUBLIC"/>
         <filter val="problem.TYPE_MAPPING_ID_CLASS_PROPERTY_METHOD_NOT_PUBLIC"/>
+        <filter val="problem.TYPE_MAPPING_MEMBER_CLASS=warning"/>
+        <filter val="problem.VIRTUAL_ATTRIBUTE_ELEMENT_COLLECTION_TARGET_CLASS_DOES_NOT_EXIST"/>
         <filter val="problem.VIRTUAL_ATTRIBUTE_EMBEDDED_ID_CLASS_SHOULD_BE_PUBLIC"/>
         <filter val="problem.VIRTUAL_ATTRIBUTE_EMBEDDED_ID_CLASS_SHOULD_IMPLEMENT_NO_ARG_CONSTRUCTOR"/>
         <filter val="problem.VIRTUAL_ATTRIBUTE_EMBEDDED_ID_CLASS_SHOULD_NOT_CONTAIN_RELATIONSHIP_MAPPINGS"/>
+        <filter val="problem.VIRTUAL_ATTRIBUTE_MAP_KEY_CLASS_MUST_BE_ENTITY_EMBEDDABLE_OR_BASIC_TYPE"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>